<commit_message>
Stashing changes before pulling updated ImageJ column
</commit_message>
<xml_diff>
--- a/raw-data/sample_info/2023-04-26_NAc_Br6522_reVisium_Summary.xlsx
+++ b/raw-data/sample_info/2023-04-26_NAc_Br6522_reVisium_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Neural_Plasticity/Molecular_Profiling/NAc/Human/N=10_Visium/2023/2023.04.26_Br6522_reVisium/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/ky/wr2b0hfd37z07ng_j240xh1w0000gq/T/ch.sudo.cyberduck/editor-ad16d467-b049-47e4-babf-1c61b2e94ee1/0c4fa306f205563f348d7eba2d3cc90f/1356240651/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5993AF6-B1FE-9343-987E-69AA701C0062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC67D2C0-A83C-704C-88E7-BE09E63DEA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33460" windowHeight="22120" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33460" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
   <si>
     <t>Sample #</t>
   </si>
@@ -132,18 +132,6 @@
   </si>
   <si>
     <t>HYP_1v_hrd</t>
-  </si>
-  <si>
-    <t>SI-TT-G9</t>
-  </si>
-  <si>
-    <t>CCGGAGGAAG</t>
-  </si>
-  <si>
-    <t>TGCGGATGTT</t>
-  </si>
-  <si>
-    <t>AACATCCGCA</t>
   </si>
   <si>
     <t>Agilent [cDNA] pg/ul</t>
@@ -243,7 +231,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -297,14 +285,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -320,7 +300,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -393,17 +373,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -415,7 +384,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,22 +437,6 @@
     <xf numFmtId="2" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,14 +484,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1126612</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>122901</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>910302</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>81935</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>81934</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1362,11 +1315,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB153"/>
+  <dimension ref="A1:AB152"/>
   <sheetViews>
-    <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3:N6"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1419,16 +1372,16 @@
         <v>10</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>11</v>
@@ -1440,13 +1393,13 @@
         <v>17</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="R1" s="12" t="s">
         <v>13</v>
@@ -1467,160 +1420,160 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="16" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="17">
-        <v>15.91</v>
-      </c>
-      <c r="G2" s="16">
+      <c r="F2" s="3">
+        <v>15.03</v>
+      </c>
+      <c r="G2" s="2">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1717.14</v>
+      </c>
+      <c r="I2" s="3">
+        <v>5</v>
+      </c>
+      <c r="J2" s="20">
+        <f>H2*I2</f>
+        <v>8585.7000000000007</v>
+      </c>
+      <c r="K2" s="20">
+        <f>(H2*I2*40)/1000</f>
+        <v>343.428</v>
+      </c>
+      <c r="L2" s="20">
+        <f>0.25*K2</f>
+        <v>85.856999999999999</v>
+      </c>
+      <c r="M2" s="2">
         <v>16</v>
       </c>
-      <c r="H2" s="16">
-        <v>1950.02</v>
-      </c>
-      <c r="I2" s="17">
-        <v>9</v>
-      </c>
-      <c r="J2" s="17">
-        <f>H2*I2</f>
-        <v>17550.18</v>
-      </c>
-      <c r="K2" s="17">
-        <f>(H2*I2*40)/1000</f>
-        <v>702.0071999999999</v>
-      </c>
-      <c r="L2" s="17">
-        <f>0.25*K2</f>
-        <v>175.50179999999997</v>
-      </c>
-      <c r="M2" s="16">
-        <v>15</v>
-      </c>
-      <c r="N2" s="16">
-        <v>443</v>
-      </c>
-      <c r="O2" s="16">
-        <v>3119.47</v>
-      </c>
-      <c r="P2" s="17">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="18">
+      <c r="N2" s="18">
+        <v>464</v>
+      </c>
+      <c r="O2" s="21">
+        <v>5814.05</v>
+      </c>
+      <c r="P2" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="22">
         <f>O2*P2</f>
-        <v>15597.349999999999</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" s="20">
-        <v>85</v>
-      </c>
-      <c r="W2" s="16">
+        <v>23256.2</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="8">
+        <v>100</v>
+      </c>
+      <c r="W2" s="23">
         <f>((V2/100)*5000*60000)</f>
-        <v>255000000</v>
-      </c>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
+        <v>300000000</v>
+      </c>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" s="3">
-        <v>15.03</v>
+        <v>14.79</v>
       </c>
       <c r="G3" s="2">
         <v>15</v>
       </c>
       <c r="H3" s="2">
-        <v>1717.14</v>
+        <v>1964.67</v>
       </c>
       <c r="I3" s="3">
-        <v>5</v>
-      </c>
-      <c r="J3" s="26">
+        <v>6</v>
+      </c>
+      <c r="J3" s="20">
         <f>H3*I3</f>
-        <v>8585.7000000000007</v>
-      </c>
-      <c r="K3" s="26">
+        <v>11788.02</v>
+      </c>
+      <c r="K3" s="20">
         <f>(H3*I3*40)/1000</f>
-        <v>343.428</v>
-      </c>
-      <c r="L3" s="26">
+        <v>471.52080000000007</v>
+      </c>
+      <c r="L3" s="20">
         <f>0.25*K3</f>
-        <v>85.856999999999999</v>
+        <v>117.88020000000002</v>
       </c>
       <c r="M3" s="2">
         <v>16</v>
       </c>
-      <c r="N3" s="24">
-        <v>464</v>
-      </c>
-      <c r="O3" s="27">
-        <v>5814.05</v>
+      <c r="N3" s="18">
+        <v>476</v>
+      </c>
+      <c r="O3" s="21">
+        <v>6175.28</v>
       </c>
       <c r="P3" s="3">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="28">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="22">
         <f>O3*P3</f>
-        <v>23256.2</v>
-      </c>
-      <c r="R3" s="24" t="s">
+        <v>18525.84</v>
+      </c>
+      <c r="R3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="S3" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="T3" s="24" t="s">
+      <c r="T3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="U3" s="24" t="s">
+      <c r="U3" s="18" t="s">
         <v>54</v>
       </c>
       <c r="V3" s="8">
-        <v>100</v>
-      </c>
-      <c r="W3" s="29">
+        <v>85</v>
+      </c>
+      <c r="W3" s="23">
         <f>((V3/100)*5000*60000)</f>
-        <v>300000000</v>
+        <v>255000000</v>
       </c>
       <c r="X3"/>
       <c r="Y3"/>
@@ -1629,78 +1582,78 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3">
-        <v>14.79</v>
+        <v>15.25</v>
       </c>
       <c r="G4" s="2">
         <v>15</v>
       </c>
       <c r="H4" s="2">
-        <v>1964.67</v>
+        <v>1785.35</v>
       </c>
       <c r="I4" s="3">
-        <v>6</v>
-      </c>
-      <c r="J4" s="26">
+        <v>5</v>
+      </c>
+      <c r="J4" s="20">
         <f>H4*I4</f>
-        <v>11788.02</v>
-      </c>
-      <c r="K4" s="26">
+        <v>8926.75</v>
+      </c>
+      <c r="K4" s="20">
         <f>(H4*I4*40)/1000</f>
-        <v>471.52080000000007</v>
-      </c>
-      <c r="L4" s="26">
+        <v>357.07</v>
+      </c>
+      <c r="L4" s="20">
         <f>0.25*K4</f>
-        <v>117.88020000000002</v>
+        <v>89.267499999999998</v>
       </c>
       <c r="M4" s="2">
         <v>16</v>
       </c>
-      <c r="N4" s="24">
-        <v>476</v>
-      </c>
-      <c r="O4" s="27">
-        <v>6175.28</v>
+      <c r="N4" s="18">
+        <v>464</v>
+      </c>
+      <c r="O4" s="21">
+        <v>7063.84</v>
       </c>
       <c r="P4" s="3">
         <v>3</v>
       </c>
-      <c r="Q4" s="28">
+      <c r="Q4" s="22">
         <f>O4*P4</f>
-        <v>18525.84</v>
-      </c>
-      <c r="R4" s="24" t="s">
+        <v>21191.52</v>
+      </c>
+      <c r="R4" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="T4" s="24" t="s">
+      <c r="T4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="18" t="s">
         <v>58</v>
       </c>
       <c r="V4" s="8">
-        <v>85</v>
-      </c>
-      <c r="W4" s="29">
+        <v>98</v>
+      </c>
+      <c r="W4" s="23">
         <f>((V4/100)*5000*60000)</f>
-        <v>255000000</v>
+        <v>294000000</v>
       </c>
       <c r="X4"/>
       <c r="Y4"/>
@@ -1709,183 +1662,103 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3">
-        <v>15.25</v>
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>15.7</v>
       </c>
       <c r="G5" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="2">
-        <v>1785.35</v>
+        <v>1470.21</v>
       </c>
       <c r="I5" s="3">
-        <v>5</v>
-      </c>
-      <c r="J5" s="26">
+        <v>8</v>
+      </c>
+      <c r="J5" s="20">
         <f>H5*I5</f>
-        <v>8926.75</v>
-      </c>
-      <c r="K5" s="26">
+        <v>11761.68</v>
+      </c>
+      <c r="K5" s="20">
         <f>(H5*I5*40)/1000</f>
-        <v>357.07</v>
-      </c>
-      <c r="L5" s="26">
+        <v>470.46719999999999</v>
+      </c>
+      <c r="L5" s="20">
         <f>0.25*K5</f>
-        <v>89.267499999999998</v>
+        <v>117.6168</v>
       </c>
       <c r="M5" s="2">
         <v>16</v>
       </c>
-      <c r="N5" s="24">
-        <v>464</v>
-      </c>
-      <c r="O5" s="27">
-        <v>7063.84</v>
-      </c>
-      <c r="P5" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="28">
+      <c r="N5" s="18">
+        <v>466</v>
+      </c>
+      <c r="O5" s="21">
+        <v>6247.93</v>
+      </c>
+      <c r="P5" s="19">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="22">
         <f>O5*P5</f>
-        <v>21191.52</v>
-      </c>
-      <c r="R5" s="24" t="s">
+        <v>24991.72</v>
+      </c>
+      <c r="R5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="S5" s="24" t="s">
+      <c r="S5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="T5" s="24" t="s">
+      <c r="T5" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="U5" s="24" t="s">
+      <c r="U5" s="18" t="s">
         <v>62</v>
       </c>
       <c r="V5" s="8">
-        <v>98</v>
-      </c>
-      <c r="W5" s="29">
+        <v>90</v>
+      </c>
+      <c r="W5" s="23">
         <f>((V5/100)*5000*60000)</f>
-        <v>294000000</v>
-      </c>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="AA5" s="10"/>
-      <c r="AB5" s="10"/>
+        <v>270000000</v>
+      </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="2">
-        <v>15.7</v>
-      </c>
-      <c r="G6" s="2">
-        <v>16</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1470.21</v>
-      </c>
-      <c r="I6" s="3">
-        <v>8</v>
-      </c>
-      <c r="J6" s="26">
-        <f>H6*I6</f>
-        <v>11761.68</v>
-      </c>
-      <c r="K6" s="26">
-        <f>(H6*I6*40)/1000</f>
-        <v>470.46719999999999</v>
-      </c>
-      <c r="L6" s="26">
-        <f>0.25*K6</f>
-        <v>117.6168</v>
-      </c>
-      <c r="M6" s="2">
-        <v>16</v>
-      </c>
-      <c r="N6" s="24">
-        <v>466</v>
-      </c>
-      <c r="O6" s="27">
-        <v>6247.93</v>
-      </c>
-      <c r="P6" s="25">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="28">
-        <f>O6*P6</f>
-        <v>24991.72</v>
-      </c>
-      <c r="R6" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="S6" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="T6" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="U6" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="V6" s="8">
-        <v>90</v>
-      </c>
-      <c r="W6" s="29">
-        <f>((V6/100)*5000*60000)</f>
-        <v>270000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="D7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="153" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="152" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1932,7 +1805,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3">
         <v>15.03</v>
@@ -1946,7 +1819,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3">
         <v>14.79</v>
@@ -1960,7 +1833,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3">
         <v>15.25</v>
@@ -1974,7 +1847,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2">
         <v>15.7</v>
@@ -2044,16 +1917,16 @@
         <v>10</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="14:24" x14ac:dyDescent="0.2">
@@ -2095,16 +1968,16 @@
     </row>
     <row r="5" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>5</v>
@@ -2121,27 +1994,27 @@
       <c r="V5" s="3">
         <v>5</v>
       </c>
-      <c r="W5" s="26">
+      <c r="W5" s="20">
         <f>U5*V5</f>
         <v>8585.7000000000007</v>
       </c>
-      <c r="X5" s="26">
+      <c r="X5" s="20">
         <f>(U5*V5*40)/1000</f>
         <v>343.428</v>
       </c>
     </row>
     <row r="6" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>6</v>
@@ -2158,27 +2031,27 @@
       <c r="V6" s="3">
         <v>6</v>
       </c>
-      <c r="W6" s="26">
+      <c r="W6" s="20">
         <f>U6*V6</f>
         <v>11788.02</v>
       </c>
-      <c r="X6" s="26">
+      <c r="X6" s="20">
         <f>(U6*V6*40)/1000</f>
         <v>471.52080000000007</v>
       </c>
     </row>
     <row r="7" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N7" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>7</v>
@@ -2195,27 +2068,27 @@
       <c r="V7" s="3">
         <v>5</v>
       </c>
-      <c r="W7" s="26">
+      <c r="W7" s="20">
         <f>U7*V7</f>
         <v>8926.75</v>
       </c>
-      <c r="X7" s="26">
+      <c r="X7" s="20">
         <f>(U7*V7*40)/1000</f>
         <v>357.07</v>
       </c>
     </row>
     <row r="8" spans="14:24" x14ac:dyDescent="0.2">
       <c r="N8" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>8</v>
@@ -2232,11 +2105,11 @@
       <c r="V8" s="3">
         <v>8</v>
       </c>
-      <c r="W8" s="26">
+      <c r="W8" s="20">
         <f>U8*V8</f>
         <v>11761.68</v>
       </c>
-      <c r="X8" s="26">
+      <c r="X8" s="20">
         <f>(U8*V8*40)/1000</f>
         <v>470.46719999999999</v>
       </c>
@@ -2271,7 +2144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14171A6-084A-884D-A0A5-4431E3FDDF37}">
   <dimension ref="B4:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="63" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="X54" sqref="X54"/>
     </sheetView>
   </sheetViews>
@@ -2281,16 +2154,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>41</v>
+      <c r="C4" s="24" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
@@ -2298,7 +2171,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" s="3">
         <v>3</v>
@@ -2306,7 +2179,7 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3">
         <v>3</v>
@@ -2314,9 +2187,9 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="25">
+        <v>45</v>
+      </c>
+      <c r="C8" s="19">
         <v>4</v>
       </c>
     </row>

</xml_diff>